<commit_message>
https submodule, update table
</commit_message>
<xml_diff>
--- a/202ki.xlsx
+++ b/202ki.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Группа</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>07.11</t>
+  </si>
+  <si>
+    <t>14.11</t>
+  </si>
+  <si>
+    <t>Групповая</t>
   </si>
   <si>
     <t xml:space="preserve">Баймухамбетова Адель</t>
@@ -223,7 +229,7 @@
       <sz val="11.000000"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,14 +262,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor rgb="FFFF7D7D"/>
+        <bgColor rgb="FFFF7D7D"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor theme="7" tint="0.59999389629810485"/>
       </patternFill>
     </fill>
     <fill>
@@ -276,6 +282,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFC7E7E"/>
         <bgColor rgb="FFFC7E7E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor theme="9" tint="0.39997558519241921"/>
       </patternFill>
     </fill>
   </fills>
@@ -301,9 +313,6 @@
     <xf fontId="3" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf fontId="3" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf fontId="3" fillId="5" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -314,9 +323,8 @@
     <xf fontId="2" fillId="6" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf fontId="2" fillId="7" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf fontId="2" fillId="7" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -324,12 +332,12 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="5" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf fontId="5" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="5" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="5" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="5" fillId="8" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="2" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf fontId="2" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="2" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="2" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -862,7 +870,8 @@
     <col customWidth="1" min="18" max="18" width="6.57421875"/>
     <col customWidth="1" min="19" max="19" width="6.00390625"/>
     <col customWidth="1" min="20" max="20" width="6.421875"/>
-    <col customWidth="1" min="21" max="21" width="7.140625"/>
+    <col customWidth="1" min="21" max="22" width="7.140625"/>
+    <col customWidth="1" min="23" max="23" width="11.140625"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5">
@@ -896,52 +905,58 @@
       <c r="L1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="S1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="U1" s="9" t="s">
         <v>17</v>
+      </c>
+      <c r="V1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="W1" s="11" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="2" ht="16.5">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1">
         <v>204</v>
       </c>
       <c r="C2" s="1">
-        <f t="shared" ref="C2:C9" si="0">SUM(J2:T2)</f>
-        <v>95</v>
+        <f t="shared" ref="C2:C9" si="0">SUM(J2:V2)</f>
+        <v>111.5</v>
       </c>
       <c r="D2" s="1">
         <f t="shared" ref="D2:D9" si="1">ROUND(C2/C$20,5)</f>
-        <v>0.65517000000000003</v>
+        <v>0.63352000000000008</v>
       </c>
       <c r="E2" s="1">
         <f t="shared" ref="E2:E9" si="2">ROUND(C$22+D$22/(E$22*D2+1),5)</f>
-        <v>7.9718800000000005</v>
+        <v>7.7892500000000009</v>
       </c>
       <c r="F2" s="1">
         <f t="shared" ref="F2:F9" si="3">ROUND(E2,0)</f>
@@ -962,7 +977,9 @@
       <c r="L2" s="12">
         <v>9</v>
       </c>
-      <c r="M2" s="12"/>
+      <c r="M2" s="12">
+        <v>0</v>
+      </c>
       <c r="N2" s="12">
         <v>12.75</v>
       </c>
@@ -984,30 +1001,36 @@
       <c r="T2" s="1">
         <v>13.5</v>
       </c>
-      <c r="U2" s="1"/>
+      <c r="U2" s="1">
+        <v>11.25</v>
+      </c>
+      <c r="V2" s="1">
+        <v>5.25</v>
+      </c>
+      <c r="W2" s="1"/>
     </row>
     <row r="3" ht="16.5">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1">
         <v>204</v>
       </c>
       <c r="C3" s="1">
         <f t="shared" si="0"/>
-        <v>73.875</v>
+        <v>86.125</v>
       </c>
       <c r="D3" s="1">
         <f t="shared" si="1"/>
-        <v>0.50948000000000004</v>
+        <v>0.48935000000000006</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" si="2"/>
-        <v>6.6769000000000007</v>
+        <v>6.4850100000000008</v>
       </c>
       <c r="F3" s="1">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1">
@@ -1024,7 +1047,9 @@
       <c r="L3" s="12">
         <v>10</v>
       </c>
-      <c r="M3" s="12"/>
+      <c r="M3" s="12">
+        <v>0</v>
+      </c>
       <c r="N3" s="12">
         <v>12.25</v>
       </c>
@@ -1044,28 +1069,32 @@
         <v>0</v>
       </c>
       <c r="T3" s="1">
-        <v>3.25</v>
-      </c>
-      <c r="U3" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="U3" s="1">
+        <v>11.5</v>
+      </c>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
     </row>
     <row r="4" ht="16.5">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1">
         <v>203</v>
       </c>
       <c r="C4" s="1">
         <f t="shared" si="0"/>
-        <v>67.625</v>
+        <v>76.375</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" si="1"/>
-        <v>0.46638000000000002</v>
+        <v>0.43395000000000006</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="2"/>
-        <v>6.2618900000000002</v>
+        <v>5.9390600000000004</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="3"/>
@@ -1086,7 +1115,9 @@
       <c r="L4" s="12">
         <v>8</v>
       </c>
-      <c r="M4" s="12"/>
+      <c r="M4" s="12">
+        <v>0</v>
+      </c>
       <c r="N4" s="12">
         <v>10.75</v>
       </c>
@@ -1106,26 +1137,30 @@
         <v>0</v>
       </c>
       <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
+      <c r="U4" s="1">
+        <v>8.75</v>
+      </c>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
     </row>
     <row r="5" ht="16.5">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1">
         <v>202</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" si="0"/>
-        <v>62.625</v>
+        <v>83.125</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="1"/>
-        <v>0.43190000000000006</v>
+        <v>0.47230000000000005</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="2"/>
-        <v>5.9183400000000006</v>
+        <v>6.3198300000000005</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="3"/>
@@ -1146,7 +1181,9 @@
       <c r="L5" s="12">
         <v>4</v>
       </c>
-      <c r="M5" s="12"/>
+      <c r="M5" s="12">
+        <v>4</v>
+      </c>
       <c r="N5" s="12">
         <v>6.5</v>
       </c>
@@ -1168,30 +1205,36 @@
       <c r="T5" s="1">
         <v>11.25</v>
       </c>
-      <c r="U5" s="1"/>
+      <c r="U5" s="1">
+        <v>8.75</v>
+      </c>
+      <c r="V5" s="1">
+        <v>7.75</v>
+      </c>
+      <c r="W5" s="1"/>
     </row>
     <row r="6" ht="16.5">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1">
         <v>201</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="0"/>
-        <v>30.5</v>
+        <v>42.75</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="1"/>
-        <v>0.21034000000000003</v>
+        <v>0.24290000000000003</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="2"/>
-        <v>3.4296100000000003</v>
+        <v>3.8291900000000001</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1">
@@ -1224,13 +1267,19 @@
         <v>2</v>
       </c>
       <c r="T6" s="1">
-        <v>1</v>
-      </c>
-      <c r="U6" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="U6" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="V6" s="1">
+        <v>4.75</v>
+      </c>
+      <c r="W6" s="1"/>
     </row>
     <row r="7" ht="16.5">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1">
         <v>201</v>
@@ -1241,11 +1290,11 @@
       </c>
       <c r="D7" s="1">
         <f t="shared" si="1"/>
-        <v>0.20086000000000001</v>
+        <v>0.16548000000000002</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="2"/>
-        <v>3.3108300000000002</v>
+        <v>2.8574100000000002</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="3"/>
@@ -1266,7 +1315,9 @@
       <c r="L7" s="12">
         <v>0</v>
       </c>
-      <c r="M7" s="12"/>
+      <c r="M7" s="12">
+        <v>0</v>
+      </c>
       <c r="N7" s="12">
         <v>8.75</v>
       </c>
@@ -1285,27 +1336,33 @@
       <c r="S7" s="1">
         <v>0</v>
       </c>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
+      <c r="T7" s="1">
+        <v>0</v>
+      </c>
+      <c r="U7" s="1">
+        <v>0</v>
+      </c>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
     </row>
     <row r="8" ht="16.5">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B8" s="1">
         <v>205</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" si="0"/>
-        <v>80.375</v>
+        <v>93.625</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="1"/>
-        <v>0.55431000000000008</v>
+        <v>0.53195999999999999</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="2"/>
-        <v>7.0924500000000004</v>
+        <v>6.8872700000000009</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="3"/>
@@ -1326,7 +1383,9 @@
       <c r="L8" s="12">
         <v>8</v>
       </c>
-      <c r="M8" s="12"/>
+      <c r="M8" s="12">
+        <v>0</v>
+      </c>
       <c r="N8" s="12">
         <v>6</v>
       </c>
@@ -1348,26 +1407,32 @@
       <c r="T8" s="1">
         <v>10</v>
       </c>
-      <c r="U8" s="1"/>
+      <c r="U8" s="1">
+        <v>9.25</v>
+      </c>
+      <c r="V8" s="1">
+        <v>4</v>
+      </c>
+      <c r="W8" s="1"/>
     </row>
     <row r="9" ht="16.5">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B9" s="1">
         <v>205</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" si="0"/>
-        <v>73.25</v>
+        <v>87.5</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="1"/>
-        <v>0.50517000000000001</v>
+        <v>0.49716000000000005</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="2"/>
-        <v>6.6361000000000008</v>
+        <v>6.5598600000000005</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="3"/>
@@ -1388,7 +1453,9 @@
       <c r="L9" s="12">
         <v>0</v>
       </c>
-      <c r="M9" s="12"/>
+      <c r="M9" s="12">
+        <v>0</v>
+      </c>
       <c r="N9" s="12">
         <v>14.25</v>
       </c>
@@ -1408,32 +1475,38 @@
         <v>0</v>
       </c>
       <c r="T9" s="1">
-        <v>5.5</v>
-      </c>
-      <c r="U9" s="1"/>
+        <v>9.5</v>
+      </c>
+      <c r="U9" s="1">
+        <v>5.25</v>
+      </c>
+      <c r="V9" s="1">
+        <v>5</v>
+      </c>
+      <c r="W9" s="1"/>
     </row>
     <row r="10" ht="16.5">
       <c r="A10" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B10" s="1">
         <v>202</v>
       </c>
       <c r="C10" s="1">
-        <f t="shared" ref="C10:C18" si="5">SUM(J10:T10)</f>
-        <v>101.75</v>
+        <f t="shared" ref="C10:C20" si="5">SUM(J10:V10)</f>
+        <v>134.25</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" ref="D10:D18" si="6">ROUND(C10/C$20,5)</f>
-        <v>0.70172000000000001</v>
+        <v>0.76278000000000001</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" ref="E10:E20" si="7">ROUND(C$22+D$22/(E$22*D10+1),5)</f>
-        <v>8.3538500000000013</v>
+        <v>8.83385</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" ref="F10:F20" si="8">ROUND(E10,0)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1">
@@ -1450,7 +1523,9 @@
       <c r="L10" s="12">
         <v>9</v>
       </c>
-      <c r="M10" s="12"/>
+      <c r="M10" s="12">
+        <v>7</v>
+      </c>
       <c r="N10" s="12">
         <v>12.25</v>
       </c>
@@ -1472,26 +1547,32 @@
       <c r="T10" s="1">
         <v>11.5</v>
       </c>
-      <c r="U10" s="1"/>
+      <c r="U10" s="1">
+        <v>13.75</v>
+      </c>
+      <c r="V10" s="1">
+        <v>11.75</v>
+      </c>
+      <c r="W10" s="1"/>
     </row>
     <row r="11" ht="16.5">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B11" s="1">
         <v>204</v>
       </c>
       <c r="C11" s="1">
         <f t="shared" si="5"/>
-        <v>68.5</v>
+        <v>77.75</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="6"/>
-        <v>0.47241000000000005</v>
+        <v>0.44176000000000004</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="7"/>
-        <v>6.3209000000000009</v>
+        <v>6.0176600000000002</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" si="8"/>
@@ -1512,7 +1593,9 @@
       <c r="L11" s="12">
         <v>0</v>
       </c>
-      <c r="M11" s="12"/>
+      <c r="M11" s="12">
+        <v>0</v>
+      </c>
       <c r="N11" s="12">
         <v>16</v>
       </c>
@@ -1532,28 +1615,34 @@
         <v>0</v>
       </c>
       <c r="T11" s="1">
-        <v>5.5</v>
-      </c>
-      <c r="U11" s="1"/>
+        <v>7.5</v>
+      </c>
+      <c r="U11" s="1">
+        <v>6.75</v>
+      </c>
+      <c r="V11" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="W11" s="1"/>
     </row>
     <row r="12" ht="16.5">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1">
         <v>202</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" si="5"/>
-        <v>33.5</v>
+        <v>42.75</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="6"/>
-        <v>0.23103000000000001</v>
+        <v>0.24290000000000003</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="7"/>
-        <v>3.6850000000000005</v>
+        <v>3.8291900000000001</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" si="8"/>
@@ -1574,7 +1663,9 @@
       <c r="L12" s="12">
         <v>0</v>
       </c>
-      <c r="M12" s="12"/>
+      <c r="M12" s="12">
+        <v>0</v>
+      </c>
       <c r="N12" s="12">
         <v>3</v>
       </c>
@@ -1594,30 +1685,34 @@
         <v>0</v>
       </c>
       <c r="T12" s="1"/>
-      <c r="U12" s="1"/>
+      <c r="U12" s="1">
+        <v>9.25</v>
+      </c>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
     </row>
     <row r="13" ht="16.5">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B13" s="1">
         <v>204</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" si="5"/>
-        <v>72</v>
+        <v>76.75</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="6"/>
-        <v>0.49655000000000005</v>
+        <v>0.43608000000000002</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="7"/>
-        <v>6.5540300000000009</v>
+        <v>5.9605500000000005</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" si="8"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1">
@@ -1634,7 +1729,9 @@
       <c r="L13" s="12">
         <v>0</v>
       </c>
-      <c r="M13" s="12"/>
+      <c r="M13" s="12">
+        <v>0</v>
+      </c>
       <c r="N13" s="12">
         <v>15</v>
       </c>
@@ -1656,30 +1753,36 @@
       <c r="T13" s="1">
         <v>3</v>
       </c>
-      <c r="U13" s="1"/>
+      <c r="U13" s="1">
+        <v>4</v>
+      </c>
+      <c r="V13" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="W13" s="1"/>
     </row>
     <row r="14" ht="16.5">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B14" s="1">
         <v>202</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" si="5"/>
-        <v>42.25</v>
+        <v>56.25</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="6"/>
-        <v>0.29138000000000003</v>
+        <v>0.31960000000000005</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="7"/>
-        <v>4.4010800000000003</v>
+        <v>4.7219300000000004</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1">
@@ -1696,7 +1799,9 @@
       <c r="L14" s="12">
         <v>0</v>
       </c>
-      <c r="M14" s="12"/>
+      <c r="M14" s="12">
+        <v>0</v>
+      </c>
       <c r="N14" s="12">
         <v>4</v>
       </c>
@@ -1716,28 +1821,32 @@
         <v>0</v>
       </c>
       <c r="T14" s="1">
-        <v>1.75</v>
-      </c>
-      <c r="U14" s="1"/>
+        <v>7.5</v>
+      </c>
+      <c r="U14" s="1">
+        <v>8.25</v>
+      </c>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
     </row>
     <row r="15" ht="16.5">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B15" s="1">
         <v>203</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" si="5"/>
-        <v>56</v>
+        <v>67.25</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="6"/>
-        <v>0.38621000000000005</v>
+        <v>0.38210000000000005</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" si="7"/>
-        <v>5.4464000000000006</v>
+        <v>5.4029800000000003</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="8"/>
@@ -1758,7 +1867,9 @@
       <c r="L15" s="12">
         <v>5</v>
       </c>
-      <c r="M15" s="12"/>
+      <c r="M15" s="12">
+        <v>0</v>
+      </c>
       <c r="N15" s="12">
         <v>6.25</v>
       </c>
@@ -1780,26 +1891,32 @@
       <c r="T15" s="1">
         <v>5</v>
       </c>
-      <c r="U15" s="1"/>
+      <c r="U15" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="V15" s="1">
+        <v>5.75</v>
+      </c>
+      <c r="W15" s="1"/>
     </row>
     <row r="16" ht="16.5">
       <c r="A16" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B16" s="1">
         <v>202</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" si="5"/>
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="6"/>
-        <v>0.40690000000000004</v>
+        <v>0.40341000000000005</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" si="7"/>
-        <v>5.6625300000000003</v>
+        <v>5.62636</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="8"/>
@@ -1820,7 +1937,9 @@
       <c r="L16" s="12">
         <v>8</v>
       </c>
-      <c r="M16" s="12"/>
+      <c r="M16" s="12">
+        <v>0</v>
+      </c>
       <c r="N16" s="12">
         <v>5</v>
       </c>
@@ -1842,30 +1961,36 @@
       <c r="T16" s="1">
         <v>5</v>
       </c>
-      <c r="U16" s="1"/>
+      <c r="U16" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="V16" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="W16" s="1"/>
     </row>
     <row r="17" ht="16.5">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B17" s="1">
         <v>204</v>
       </c>
       <c r="C17" s="1">
         <f t="shared" si="5"/>
-        <v>56.125</v>
+        <v>81.625</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" si="6"/>
-        <v>0.38707000000000003</v>
+        <v>0.46378000000000003</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" si="7"/>
-        <v>5.45547</v>
+        <v>6.2363500000000007</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1">
@@ -1882,7 +2007,9 @@
       <c r="L17" s="12">
         <v>4</v>
       </c>
-      <c r="M17" s="12"/>
+      <c r="M17" s="12">
+        <v>2</v>
+      </c>
       <c r="N17" s="12">
         <v>10.5</v>
       </c>
@@ -1902,28 +2029,34 @@
         <v>0</v>
       </c>
       <c r="T17" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="U17" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="U17" s="1">
+        <v>10.25</v>
+      </c>
+      <c r="V17" s="1">
+        <v>6.75</v>
+      </c>
+      <c r="W17" s="1"/>
     </row>
     <row r="18" ht="16.5">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B18" s="1">
         <v>203</v>
       </c>
       <c r="C18" s="1">
         <f t="shared" si="5"/>
-        <v>35.75</v>
+        <v>47.5</v>
       </c>
       <c r="D18" s="1">
         <f t="shared" si="6"/>
-        <v>0.24655000000000002</v>
+        <v>0.26989000000000002</v>
       </c>
       <c r="E18" s="1">
         <f t="shared" si="7"/>
-        <v>3.8731900000000001</v>
+        <v>4.1508799999999999</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" si="8"/>
@@ -1944,7 +2077,9 @@
       <c r="L18" s="12">
         <v>0</v>
       </c>
-      <c r="M18" s="12"/>
+      <c r="M18" s="12">
+        <v>0</v>
+      </c>
       <c r="N18" s="12">
         <v>2.25</v>
       </c>
@@ -1966,7 +2101,13 @@
       <c r="T18" s="1">
         <v>1.5</v>
       </c>
-      <c r="U18" s="1"/>
+      <c r="U18" s="1">
+        <v>7.75</v>
+      </c>
+      <c r="V18" s="1">
+        <v>4</v>
+      </c>
+      <c r="W18" s="1"/>
     </row>
     <row r="19" ht="16.5">
       <c r="A19" s="1"/>
@@ -1990,17 +2131,19 @@
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
     </row>
     <row r="20" ht="16.5">
       <c r="A20" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B20" s="1">
         <v>205</v>
       </c>
       <c r="C20" s="1">
-        <f>SUM(J20:T20)</f>
-        <v>145</v>
+        <f t="shared" si="5"/>
+        <v>176</v>
       </c>
       <c r="D20" s="1">
         <f>C20/C$20</f>
@@ -2055,6 +2198,12 @@
       </c>
       <c r="U20" s="1">
         <v>16</v>
+      </c>
+      <c r="V20" s="1">
+        <v>15</v>
+      </c>
+      <c r="W20" s="1">
+        <v>40</v>
       </c>
     </row>
     <row r="21" ht="14.25">
@@ -2065,10 +2214,10 @@
     </row>
     <row r="22" ht="16.5">
       <c r="A22" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C22" s="1">
         <v>28.5</v>
@@ -2091,16 +2240,16 @@
     <row r="23" ht="16.5">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -2114,78 +2263,78 @@
     </row>
     <row r="25" ht="16.5">
       <c r="A25" s="15" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B25" s="1"/>
     </row>
     <row r="26" ht="14.25">
       <c r="A26" s="16" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" ht="14.25">
       <c r="A27" s="16" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" ht="14.25">
       <c r="A28" s="17" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" ht="14.25">
       <c r="A29" s="17" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" ht="14.25">
       <c r="A30" s="18" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" ht="14.25">
       <c r="A31" s="18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" ht="14.25">
       <c r="A32" s="18" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" ht="14.25">
       <c r="A33" s="19" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" ht="14.25">
       <c r="A34" s="19" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" ht="14.25">
       <c r="A35" s="19" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" ht="16.5">
       <c r="A37" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" ht="16.5">
       <c r="A38" s="20" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" ht="16.5">
       <c r="A39" s="21" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" ht="16.5">
       <c r="A40" s="22" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -2198,7 +2347,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="4" operator="between" id="{00560083-009A-4BF9-BB53-002300E200FB}">
+          <x14:cfRule type="cellIs" priority="4" operator="between" id="{000000C6-000A-48FC-8E8F-001C007400D2}">
             <xm:f>3</xm:f>
             <xm:f>4</xm:f>
             <x14:dxf>
@@ -2213,7 +2362,7 @@
           <xm:sqref>F2:F18</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="between" id="{0048001D-0010-4672-A041-00890066003B}">
+          <x14:cfRule type="cellIs" priority="3" operator="between" id="{002C0005-0016-43A3-B3EA-00C700C900DB}">
             <xm:f>5</xm:f>
             <xm:f>7</xm:f>
             <x14:dxf>
@@ -2231,7 +2380,7 @@
           <xm:sqref>F2:F18</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="2" operator="between" id="{006D0049-00FB-49DE-B3C0-00F6001E0000}">
+          <x14:cfRule type="cellIs" priority="2" operator="between" id="{009700A9-000A-445C-B07A-000100EC0038}">
             <xm:f>8</xm:f>
             <xm:f>10</xm:f>
             <x14:dxf>
@@ -2246,7 +2395,7 @@
           <xm:sqref>F2:F18</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="1" operator="between" id="{003A005F-00D1-4B3F-8434-00D90082000B}">
+          <x14:cfRule type="cellIs" priority="1" operator="between" id="{00D6005B-00AE-4C04-9163-0092006A002D}">
             <xm:f>0</xm:f>
             <xm:f>2</xm:f>
             <x14:dxf>

</xml_diff>